<commit_message>
maj matrix avec IA image (bcp de value encore a NaN)
</commit_message>
<xml_diff>
--- a/ai_sustainability/datas/Weight_matrix.xlsx
+++ b/ai_sustainability/datas/Weight_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hennecarta\Documents\Graph_decision_AI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493A6789-CF79-4A41-A365-EE85DCA5A891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92CBE40-2208-42AF-AA43-19482C3F012B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AC26B5E7-4148-4700-AAF1-8A62823EFFAF}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{AC26B5E7-4148-4700-AAF1-8A62823EFFAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="101">
   <si>
     <t>id_edges</t>
   </si>
@@ -324,6 +324,21 @@
   </si>
   <si>
     <t>Gradient Boosting Machine (LightGBM) with binary crossentropy loss for classification</t>
+  </si>
+  <si>
+    <t>MobileNetV3Small</t>
+  </si>
+  <si>
+    <t>RegNetY080</t>
+  </si>
+  <si>
+    <t>ConvNeXtSmall</t>
+  </si>
+  <si>
+    <t>EfficientNetB0</t>
+  </si>
+  <si>
+    <t>EfficientNetV2S</t>
   </si>
 </sst>
 </file>
@@ -692,19 +707,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65B3A90E-CD1F-4942-85BC-B8033B44D3A6}">
-  <dimension ref="A1:X41"/>
+  <dimension ref="A1:AD41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.21875" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.5546875" style="2" customWidth="1"/>
+    <col min="25" max="30" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -777,8 +793,23 @@
       <c r="X1" t="s">
         <v>20</v>
       </c>
+      <c r="Y1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -851,8 +882,23 @@
       <c r="X2">
         <v>1</v>
       </c>
+      <c r="Y2" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -925,8 +971,23 @@
       <c r="X3">
         <v>1</v>
       </c>
+      <c r="Y3" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -999,8 +1060,23 @@
       <c r="X4">
         <v>0</v>
       </c>
+      <c r="Y4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -1073,8 +1149,23 @@
       <c r="X5">
         <v>1</v>
       </c>
+      <c r="Y5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1147,8 +1238,23 @@
       <c r="X6">
         <v>0</v>
       </c>
+      <c r="Y6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -1221,8 +1327,23 @@
       <c r="X7">
         <v>0</v>
       </c>
+      <c r="Y7" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -1295,8 +1416,23 @@
       <c r="X8">
         <v>0</v>
       </c>
+      <c r="Y8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -1369,8 +1505,23 @@
       <c r="X9">
         <v>1</v>
       </c>
+      <c r="Y9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -1443,8 +1594,23 @@
       <c r="X10">
         <v>1</v>
       </c>
+      <c r="Y10" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -1517,8 +1683,23 @@
       <c r="X11">
         <v>0</v>
       </c>
+      <c r="Y11" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
@@ -1591,8 +1772,23 @@
       <c r="X12">
         <v>0</v>
       </c>
+      <c r="Y12" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>38</v>
       </c>
@@ -1678,8 +1874,23 @@
       <c r="X13">
         <v>0</v>
       </c>
+      <c r="Y13" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -1752,8 +1963,23 @@
       <c r="X14">
         <v>1</v>
       </c>
+      <c r="Y14" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB14" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
@@ -1826,8 +2052,23 @@
       <c r="X15">
         <v>1</v>
       </c>
+      <c r="Y15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC15" s="3" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>66</v>
       </c>
@@ -1900,8 +2141,23 @@
       <c r="X16">
         <v>1</v>
       </c>
+      <c r="Y16" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB16" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC16" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
@@ -1974,8 +2230,23 @@
       <c r="X17">
         <v>0.87656656419957435</v>
       </c>
+      <c r="Y17" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z17" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA17" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB17" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC17" s="3" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
@@ -2048,8 +2319,23 @@
       <c r="X18">
         <v>0.86491557223264537</v>
       </c>
+      <c r="Y18" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z18" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA18" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB18" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC18" s="3" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
@@ -2122,8 +2408,23 @@
       <c r="X19">
         <v>0.54168452777777776</v>
       </c>
+      <c r="Y19" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z19" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA19" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB19" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC19" s="3" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>45</v>
       </c>
@@ -2196,8 +2497,23 @@
       <c r="X20">
         <v>0</v>
       </c>
+      <c r="Y20" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC20" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -2270,8 +2586,23 @@
       <c r="X21">
         <v>0</v>
       </c>
+      <c r="Y21" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB21" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC21" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
@@ -2344,8 +2675,23 @@
       <c r="X22">
         <v>0</v>
       </c>
+      <c r="Y22" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z22" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB22" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC22" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
@@ -2418,8 +2764,23 @@
       <c r="X23">
         <v>0</v>
       </c>
+      <c r="Y23" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>48</v>
       </c>
@@ -2492,8 +2853,23 @@
       <c r="X24">
         <v>0</v>
       </c>
+      <c r="Y24" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
@@ -2566,8 +2942,23 @@
       <c r="X25">
         <v>0</v>
       </c>
+      <c r="Y25" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
@@ -2640,8 +3031,23 @@
       <c r="X26">
         <v>0.6</v>
       </c>
+      <c r="Y26" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z26" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA26" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB26" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC26" s="3" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>51</v>
       </c>
@@ -2736,8 +3142,23 @@
         <f t="shared" si="2"/>
         <v>0.32501071666666664</v>
       </c>
+      <c r="Y27" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z27" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA27" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB27" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC27" s="3" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>52</v>
       </c>
@@ -2810,8 +3231,23 @@
       <c r="X28">
         <v>0.54168452777777776</v>
       </c>
+      <c r="Y28" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z28" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA28" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB28" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC28" s="3" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>59</v>
       </c>
@@ -2884,8 +3320,23 @@
       <c r="X29">
         <v>1</v>
       </c>
+      <c r="Y29" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z29" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB29" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC29" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
@@ -2958,8 +3409,23 @@
       <c r="X30">
         <v>1</v>
       </c>
+      <c r="Y30" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z30" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA30" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB30" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC30" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>54</v>
       </c>
@@ -3032,8 +3498,23 @@
       <c r="X31">
         <v>1</v>
       </c>
+      <c r="Y31" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC31" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>55</v>
       </c>
@@ -3106,8 +3587,23 @@
       <c r="X32">
         <v>1</v>
       </c>
+      <c r="Y32" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z32" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA32" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB32" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC32" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>56</v>
       </c>
@@ -3180,8 +3676,23 @@
       <c r="X33">
         <v>1</v>
       </c>
+      <c r="Y33" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z33" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA33" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB33" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC33" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>57</v>
       </c>
@@ -3254,8 +3765,23 @@
       <c r="X34">
         <v>1</v>
       </c>
+      <c r="Y34" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z34" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA34" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB34" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC34" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>58</v>
       </c>
@@ -3328,8 +3854,23 @@
       <c r="X35">
         <v>1</v>
       </c>
+      <c r="Y35" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z35" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA35" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB35" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC35" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>60</v>
       </c>
@@ -3402,8 +3943,23 @@
       <c r="X36">
         <v>1</v>
       </c>
+      <c r="Y36" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z36" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA36" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB36" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC36" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>61</v>
       </c>
@@ -3476,8 +4032,23 @@
       <c r="X37">
         <v>1</v>
       </c>
+      <c r="Y37" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z37" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA37" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB37" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC37" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>62</v>
       </c>
@@ -3550,8 +4121,23 @@
       <c r="X38">
         <v>1</v>
       </c>
+      <c r="Y38" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z38" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA38" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB38" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC38" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>63</v>
       </c>
@@ -3624,8 +4210,23 @@
       <c r="X39">
         <v>1</v>
       </c>
+      <c r="Y39" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z39" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA39" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB39" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC39" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>64</v>
       </c>
@@ -3698,8 +4299,23 @@
       <c r="X40">
         <v>1</v>
       </c>
+      <c r="Y40" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z40" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA40" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB40" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC40" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>65</v>
       </c>
@@ -3770,6 +4386,21 @@
         <v>1</v>
       </c>
       <c r="X41">
+        <v>1</v>
+      </c>
+      <c r="Y41" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z41" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA41" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB41" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC41" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modif matrix et les .json et dbconnection
</commit_message>
<xml_diff>
--- a/ai_sustainability/datas/Weight_matrix.xlsx
+++ b/ai_sustainability/datas/Weight_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hennecarta\Documents\Graph_decision_AI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2B829B-9FC9-4283-AD6A-348A10AFBE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE64586E-E81A-4B5F-949E-4150CF78200A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{AC26B5E7-4148-4700-AAF1-8A62823EFFAF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AC26B5E7-4148-4700-AAF1-8A62823EFFAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -865,7 +865,7 @@
   <dimension ref="A1:BE41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2613,43 +2613,43 @@
         <v>70</v>
       </c>
       <c r="C11">
-        <v>0.69875000000000009</v>
+        <v>0.38397624332593427</v>
       </c>
       <c r="D11">
-        <v>0.90125000000000011</v>
+        <v>0.80570241691842903</v>
       </c>
       <c r="E11">
-        <v>0.36916666666666675</v>
+        <v>0.72379283048739118</v>
       </c>
       <c r="F11">
-        <v>0.89083333333333337</v>
+        <v>0.86155606407322649</v>
       </c>
       <c r="G11">
-        <v>0.36916666666666698</v>
+        <v>0.72134565535895412</v>
       </c>
       <c r="H11">
-        <v>0.82208333333333339</v>
+        <v>0.79223913850724093</v>
       </c>
       <c r="I11">
-        <v>0.84958333333333336</v>
+        <v>0.93547208418591055</v>
       </c>
       <c r="J11">
-        <v>0.92958333333333332</v>
+        <v>0.88197602315006185</v>
       </c>
       <c r="K11">
-        <v>0.90416666666666667</v>
+        <v>0.93410683012259177</v>
       </c>
       <c r="L11">
-        <v>1</v>
+        <v>0.89504964340651649</v>
       </c>
       <c r="M11">
-        <v>0.98875000000000002</v>
+        <v>0.92599826388888862</v>
       </c>
       <c r="N11">
-        <v>0.87333333333333329</v>
+        <v>0.97153916211293256</v>
       </c>
       <c r="O11">
-        <v>0.98625000000000007</v>
+        <v>1</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -2786,43 +2786,43 @@
         <v>71</v>
       </c>
       <c r="C12">
-        <v>0.57032645000000004</v>
+        <v>0.36910994764397914</v>
       </c>
       <c r="D12">
-        <v>0.96421844999999995</v>
+        <v>0.64090909090909109</v>
       </c>
       <c r="E12">
-        <v>0.66134511666666662</v>
+        <v>0.21837893649974191</v>
       </c>
       <c r="F12">
-        <v>0.96346894999999999</v>
+        <v>0.61751824817518275</v>
       </c>
       <c r="G12">
-        <v>0.66134511666666662</v>
+        <v>0.21837893649974191</v>
       </c>
       <c r="H12">
-        <v>0.94884511666666671</v>
+        <v>0.4976470588235295</v>
       </c>
       <c r="I12">
-        <v>0.97717845000000003</v>
+        <v>0.53954081632653073</v>
       </c>
       <c r="J12">
-        <v>0.99062286666666666</v>
+        <v>0.71452702702702697</v>
       </c>
       <c r="K12">
-        <v>0.96891444999999998</v>
+        <v>0.64777947932618685</v>
       </c>
       <c r="L12">
-        <v>0.99506003333333304</v>
+        <v>1</v>
       </c>
       <c r="M12">
-        <v>1</v>
+        <v>0.94</v>
       </c>
       <c r="N12">
-        <v>0.96574611666666699</v>
+        <v>0.58184319119669881</v>
       </c>
       <c r="O12">
-        <v>0.99590986666666703</v>
+        <v>0.92763157894736858</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -2959,56 +2959,56 @@
         <v>72</v>
       </c>
       <c r="C13">
-        <f>(C12+C11)/2</f>
-        <v>0.63453822500000001</v>
+        <f>C12*C11</f>
+        <v>0.14172945107056739</v>
       </c>
       <c r="D13">
-        <f t="shared" ref="D13:O13" si="0">(D12+D11)/2</f>
-        <v>0.93273422500000003</v>
+        <f t="shared" ref="D13:O13" si="0">D12*D11</f>
+        <v>0.51638200357044783</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>0.51525589166666674</v>
+        <v>0.15806110856797445</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>0.92715114166666668</v>
+        <v>0.53202659139120434</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>0.51525589166666674</v>
+        <v>0.15752669706599776</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>0.88546422499999999</v>
+        <v>0.39425547716301523</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>0.91338089166666669</v>
+        <v>0.50472537195234723</v>
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>0.96010309999999999</v>
+        <v>0.63019570573053396</v>
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>0.93654055833333327</v>
+        <v>0.60509523605184734</v>
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>0.99753001666666652</v>
+        <v>0.89504964340651649</v>
       </c>
       <c r="M13">
         <f t="shared" si="0"/>
-        <v>0.99437500000000001</v>
+        <v>0.8704383680555553</v>
       </c>
       <c r="N13">
         <f t="shared" si="0"/>
-        <v>0.91953972500000014</v>
+        <v>0.56528344645635553</v>
       </c>
       <c r="O13">
         <f t="shared" si="0"/>
-        <v>0.99107993333333355</v>
+        <v>0.92763157894736858</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -5221,43 +5221,43 @@
         <v>79</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0.90489913544668577</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0.46176470588235291</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>0.48307692307692307</v>
       </c>
       <c r="G26">
-        <v>0.9</v>
+        <v>0.94864048338368567</v>
       </c>
       <c r="H26">
-        <v>0.3</v>
+        <v>2.3903775883069429E-2</v>
       </c>
       <c r="I26">
-        <v>0.2</v>
+        <v>6.7924201782469497E-3</v>
       </c>
       <c r="J26">
-        <v>0.6</v>
+        <v>0.60617760617760619</v>
       </c>
       <c r="K26">
-        <v>0.9</v>
+        <v>0.35885714285714282</v>
       </c>
       <c r="L26">
-        <v>1</v>
+        <v>0.18416422287390027</v>
       </c>
       <c r="M26">
-        <v>1</v>
+        <v>0.7302325581395348</v>
       </c>
       <c r="N26">
-        <v>1</v>
+        <v>0.59133709981167604</v>
       </c>
       <c r="O26">
-        <v>0.6</v>
+        <v>2.7689594356261022E-2</v>
       </c>
       <c r="P26">
         <v>0.9</v>
@@ -5395,55 +5395,55 @@
       </c>
       <c r="C27">
         <f>C26*C13</f>
-        <v>0.63453822500000001</v>
+        <v>0.1282508577410898</v>
       </c>
       <c r="D27">
         <f t="shared" ref="D27:O27" si="1">D26*D13</f>
-        <v>0.93273422500000003</v>
+        <v>0.23844698400164796</v>
       </c>
       <c r="E27">
         <f t="shared" si="1"/>
-        <v>0.51525589166666674</v>
+        <v>0.15806110856797445</v>
       </c>
       <c r="F27">
         <f t="shared" si="1"/>
-        <v>0.92715114166666668</v>
+        <v>0.25700976876436638</v>
       </c>
       <c r="G27">
         <f t="shared" si="1"/>
-        <v>0.46373030250000008</v>
+        <v>0.14943620205052352</v>
       </c>
       <c r="H27">
         <f t="shared" si="1"/>
-        <v>0.2656392675</v>
+        <v>9.4241945667773129E-3</v>
       </c>
       <c r="I27">
         <f t="shared" si="1"/>
-        <v>0.18267617833333336</v>
+        <v>3.4283068009223205E-3</v>
       </c>
       <c r="J27">
         <f t="shared" si="1"/>
-        <v>0.57606185999999993</v>
+        <v>0.3820105243231422</v>
       </c>
       <c r="K27">
         <f t="shared" si="1"/>
-        <v>0.84288650249999997</v>
+        <v>0.21714274756603433</v>
       </c>
       <c r="L27">
         <f t="shared" si="1"/>
-        <v>0.99753001666666652</v>
+        <v>0.16483612201152267</v>
       </c>
       <c r="M27">
         <f t="shared" si="1"/>
-        <v>0.99437500000000001</v>
+        <v>0.63562243620801007</v>
       </c>
       <c r="N27">
         <f t="shared" si="1"/>
-        <v>0.91953972500000014</v>
+        <v>0.33427307379905014</v>
       </c>
       <c r="O27">
         <f t="shared" si="1"/>
-        <v>0.59464796000000009</v>
+        <v>2.5685742133110558E-2</v>
       </c>
       <c r="P27">
         <f t="shared" ref="P27:AC27" si="2">P26*P28</f>
@@ -5614,43 +5614,56 @@
         <v>81</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <f>C13</f>
+        <v>0.14172945107056739</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <f t="shared" ref="D28:O28" si="12">D13</f>
+        <v>0.51638200357044783</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <f t="shared" si="12"/>
+        <v>0.15806110856797445</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <f t="shared" si="12"/>
+        <v>0.53202659139120434</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <f t="shared" si="12"/>
+        <v>0.15752669706599776</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <f t="shared" si="12"/>
+        <v>0.39425547716301523</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <f t="shared" si="12"/>
+        <v>0.50472537195234723</v>
       </c>
       <c r="J28">
-        <v>1</v>
+        <f t="shared" si="12"/>
+        <v>0.63019570573053396</v>
       </c>
       <c r="K28">
-        <v>1</v>
+        <f t="shared" si="12"/>
+        <v>0.60509523605184734</v>
       </c>
       <c r="L28">
-        <v>1</v>
+        <f t="shared" si="12"/>
+        <v>0.89504964340651649</v>
       </c>
       <c r="M28">
-        <v>1</v>
+        <f t="shared" si="12"/>
+        <v>0.8704383680555553</v>
       </c>
       <c r="N28">
-        <v>1</v>
+        <f t="shared" si="12"/>
+        <v>0.56528344645635553</v>
       </c>
       <c r="O28">
-        <v>1</v>
+        <f t="shared" si="12"/>
+        <v>0.92763157894736858</v>
       </c>
       <c r="P28">
         <v>0.46468986111111116</v>
@@ -5702,19 +5715,19 @@
         <v>0.97563025210084031</v>
       </c>
       <c r="AF28" s="3">
-        <f t="shared" ref="AF28:AI28" si="12">AF21</f>
+        <f t="shared" ref="AF28:AI28" si="13">AF21</f>
         <v>1</v>
       </c>
       <c r="AG28" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.83697478991596641</v>
       </c>
       <c r="AH28" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.754621848739496</v>
       </c>
       <c r="AI28" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.62016806722689077</v>
       </c>
       <c r="AJ28">
@@ -5722,27 +5735,27 @@
         <v>1</v>
       </c>
       <c r="AK28">
-        <f t="shared" ref="AK28:AP28" si="13">AK22</f>
+        <f t="shared" ref="AK28:AP28" si="14">AK22</f>
         <v>0.77439797211660322</v>
       </c>
       <c r="AL28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.56147021546261078</v>
       </c>
       <c r="AM28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.83269961977186313</v>
       </c>
       <c r="AN28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.71482889733840294</v>
       </c>
       <c r="AO28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.94169835234474009</v>
       </c>
       <c r="AP28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.64892268694550059</v>
       </c>
       <c r="AQ28">
@@ -5750,27 +5763,27 @@
         <v>0.78797083839611193</v>
       </c>
       <c r="AR28">
-        <f t="shared" ref="AR28:AW28" si="14">AR23</f>
+        <f t="shared" ref="AR28:AW28" si="15">AR23</f>
         <v>0.81206966383151069</v>
       </c>
       <c r="AS28">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.92831105710814099</v>
       </c>
       <c r="AT28">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="AU28">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.98541919805589306</v>
       </c>
       <c r="AV28">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.87140542729850157</v>
       </c>
       <c r="AW28">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.89712434183880108</v>
       </c>
       <c r="AX28" s="3">

</xml_diff>

<commit_message>
debut de la partie 2 du form
deja fait :
* ajout des metrics dans le graph
* creation d'une experiment mlflow quand un graph est save
* affichage de l'ID dans form et history
* modif de la matrice des poids avec les metrics
</commit_message>
<xml_diff>
--- a/ai_sustainability/datas/Weight_matrix.xlsx
+++ b/ai_sustainability/datas/Weight_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hennecarta\Documents\Graph_decision_AI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE64586E-E81A-4B5F-949E-4150CF78200A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C06511-6686-48C3-943D-DB31FA99B283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AC26B5E7-4148-4700-AAF1-8A62823EFFAF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="136">
   <si>
     <t>id_edges</t>
   </si>
@@ -248,21 +248,9 @@
     <t>Classify between two choices</t>
   </si>
   <si>
-    <t>Minimize the maximum error that can be made.</t>
-  </si>
-  <si>
-    <t>Minimize the average error.</t>
-  </si>
-  <si>
     <t>Balanced</t>
   </si>
   <si>
-    <t>That a true thing is considered false.</t>
-  </si>
-  <si>
-    <t>That a false thing is considered true.</t>
-  </si>
-  <si>
     <t>Object detection</t>
   </si>
   <si>
@@ -359,9 +347,6 @@
     <t>YOLOX</t>
   </si>
   <si>
-    <t>LightGBM for image (only small dataset)</t>
-  </si>
-  <si>
     <t>Regnety080</t>
   </si>
   <si>
@@ -408,6 +393,57 @@
   </si>
   <si>
     <t>BP-RNN</t>
+  </si>
+  <si>
+    <t>metric</t>
+  </si>
+  <si>
+    <t>f1_score_handmade</t>
+  </si>
+  <si>
+    <t>max_error</t>
+  </si>
+  <si>
+    <t>mean_absolute_error</t>
+  </si>
+  <si>
+    <t>Minimize the average error</t>
+  </si>
+  <si>
+    <t>Minimize the maximum error that can be made</t>
+  </si>
+  <si>
+    <t>That a false thing is considered true</t>
+  </si>
+  <si>
+    <t>That a true thing is considered false</t>
+  </si>
+  <si>
+    <t>max_error,mean_absolute_error</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Duration,Accuracy</t>
+  </si>
+  <si>
+    <t>false_negatives</t>
+  </si>
+  <si>
+    <t>false_positives</t>
+  </si>
+  <si>
+    <t>f1_score</t>
+  </si>
+  <si>
+    <t>evaluation_accuracy</t>
+  </si>
+  <si>
+    <t>LightGBM for image (only small dataset: less than 5000 samples)</t>
   </si>
 </sst>
 </file>
@@ -862,201 +898,205 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65B3A90E-CD1F-4942-85BC-B8033B44D3A6}">
-  <dimension ref="A1:BE41"/>
+  <dimension ref="A1:BF41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.21875" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" customWidth="1"/>
     <col min="25" max="30" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>1</v>
+      <c r="C1" t="s">
+        <v>119</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA1" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="AC1" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="W1" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="X1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y1" s="11" t="s">
+      <c r="AD1" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE1" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="AF1" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="AG1" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AH1" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI1" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ1" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="AK1" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="Z1" s="11" t="s">
+      <c r="AL1" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="AA1" s="11" t="s">
+      <c r="AM1" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="AB1" s="11" t="s">
+      <c r="AN1" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="AC1" s="12" t="s">
+      <c r="AO1" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="AP1" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ1" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="AR1" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="AS1" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="AT1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="AU1" s="13" t="s">
         <v>108</v>
-      </c>
-      <c r="AD1" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="AE1" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="AF1" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="AG1" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="AH1" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI1" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="AJ1" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="AK1" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="AL1" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="AM1" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="AN1" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="AO1" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="AP1" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="AQ1" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="AR1" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="AS1" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="AT1" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="AU1" s="13" t="s">
-        <v>114</v>
       </c>
       <c r="AV1" s="13" t="s">
         <v>109</v>
       </c>
       <c r="AW1" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="AX1" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="AY1" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="AZ1" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="BA1" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB1" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="BC1" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="AX1" s="14" t="s">
+      <c r="BD1" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="AY1" s="14" t="s">
+      <c r="BE1" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="AZ1" s="14" t="s">
+      <c r="BF1" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="BA1" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="BB1" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="BC1" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="BD1" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="BE1" s="15" t="s">
-        <v>123</v>
-      </c>
     </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
+        <v>89</v>
+      </c>
+      <c r="C2" t="s">
+        <v>89</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1121,7 +1161,7 @@
       <c r="X2">
         <v>1</v>
       </c>
-      <c r="Y2" s="3">
+      <c r="Y2">
         <v>1</v>
       </c>
       <c r="Z2" s="3">
@@ -1220,16 +1260,19 @@
       <c r="BE2" s="3">
         <v>1</v>
       </c>
+      <c r="BF2" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C3">
-        <v>1</v>
+      <c r="C3" t="s">
+        <v>89</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1294,7 +1337,7 @@
       <c r="X3">
         <v>1</v>
       </c>
-      <c r="Y3" s="3">
+      <c r="Y3">
         <v>1</v>
       </c>
       <c r="Z3" s="3">
@@ -1393,21 +1436,24 @@
       <c r="BE3" s="3">
         <v>1</v>
       </c>
+      <c r="BF3" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="C4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
         <v>1</v>
       </c>
       <c r="F4" s="4">
@@ -1416,11 +1462,11 @@
       <c r="G4" s="4">
         <v>1</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <v>1</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -1441,10 +1487,10 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -1467,7 +1513,7 @@
       <c r="X4">
         <v>0</v>
       </c>
-      <c r="Y4" s="3">
+      <c r="Y4">
         <v>0</v>
       </c>
       <c r="Z4" s="3">
@@ -1531,10 +1577,10 @@
         <v>0</v>
       </c>
       <c r="AT4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV4" s="3">
         <v>0</v>
@@ -1566,16 +1612,19 @@
       <c r="BE4" s="3">
         <v>0</v>
       </c>
+      <c r="BF4" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C5">
-        <v>1</v>
+      <c r="C5" t="s">
+        <v>89</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1583,10 +1632,10 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5" s="5">
-        <v>1</v>
-      </c>
-      <c r="G5">
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
         <v>1</v>
       </c>
       <c r="H5">
@@ -1640,8 +1689,8 @@
       <c r="X5">
         <v>1</v>
       </c>
-      <c r="Y5" s="3">
-        <v>0</v>
+      <c r="Y5">
+        <v>1</v>
       </c>
       <c r="Z5" s="3">
         <v>0</v>
@@ -1739,16 +1788,19 @@
       <c r="BE5" s="3">
         <v>0</v>
       </c>
+      <c r="BF5" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C6">
-        <v>0</v>
+      <c r="C6" t="s">
+        <v>89</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1813,7 +1865,7 @@
       <c r="X6">
         <v>0</v>
       </c>
-      <c r="Y6" s="3">
+      <c r="Y6">
         <v>0</v>
       </c>
       <c r="Z6" s="3">
@@ -1868,7 +1920,7 @@
         <v>0</v>
       </c>
       <c r="AQ6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR6" s="3">
         <v>1</v>
@@ -1912,16 +1964,19 @@
       <c r="BE6" s="3">
         <v>1</v>
       </c>
+      <c r="BF6" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C7">
-        <v>0</v>
+      <c r="C7" t="s">
+        <v>89</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1986,8 +2041,8 @@
       <c r="X7">
         <v>0</v>
       </c>
-      <c r="Y7" s="3">
-        <v>1</v>
+      <c r="Y7">
+        <v>0</v>
       </c>
       <c r="Z7" s="3">
         <v>1</v>
@@ -2041,7 +2096,7 @@
         <v>1</v>
       </c>
       <c r="AQ7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR7" s="3">
         <v>0</v>
@@ -2085,16 +2140,19 @@
       <c r="BE7" s="3">
         <v>0</v>
       </c>
+      <c r="BF7" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C8">
-        <v>1</v>
+      <c r="C8" t="s">
+        <v>89</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2133,7 +2191,7 @@
         <v>1</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8">
         <v>0</v>
@@ -2159,7 +2217,7 @@
       <c r="X8">
         <v>0</v>
       </c>
-      <c r="Y8" s="3">
+      <c r="Y8">
         <v>0</v>
       </c>
       <c r="Z8" s="3">
@@ -2258,16 +2316,19 @@
       <c r="BE8" s="3">
         <v>0</v>
       </c>
+      <c r="BF8" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C9">
-        <v>0</v>
+      <c r="C9" t="s">
+        <v>120</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -2306,34 +2367,34 @@
         <v>0</v>
       </c>
       <c r="P9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q9">
-        <v>1</v>
+        <v>0.46468986111111099</v>
       </c>
       <c r="R9">
-        <v>1</v>
+        <v>0.51031225694444438</v>
       </c>
       <c r="S9">
-        <v>1</v>
+        <v>0.52973999999999988</v>
       </c>
       <c r="T9">
-        <v>1</v>
+        <v>0.45403111111111122</v>
       </c>
       <c r="U9">
-        <v>1</v>
+        <v>0.52557581249999985</v>
       </c>
       <c r="V9">
-        <v>1</v>
+        <v>0.54629152777777779</v>
       </c>
       <c r="W9">
-        <v>1</v>
+        <v>0.54629152777777779</v>
       </c>
       <c r="X9">
-        <v>1</v>
-      </c>
-      <c r="Y9" s="3">
-        <v>0</v>
+        <v>0.36465800000000009</v>
+      </c>
+      <c r="Y9">
+        <v>0.54168452777777776</v>
       </c>
       <c r="Z9" s="3">
         <v>0</v>
@@ -2431,16 +2492,19 @@
       <c r="BE9" s="3">
         <v>0</v>
       </c>
+      <c r="BF9" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C10">
-        <v>0</v>
+      <c r="C10" t="s">
+        <v>89</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -2479,7 +2543,7 @@
         <v>0</v>
       </c>
       <c r="P10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q10">
         <v>1</v>
@@ -2505,8 +2569,8 @@
       <c r="X10">
         <v>1</v>
       </c>
-      <c r="Y10" s="3">
-        <v>0</v>
+      <c r="Y10">
+        <v>1</v>
       </c>
       <c r="Z10" s="3">
         <v>0</v>
@@ -2604,55 +2668,58 @@
       <c r="BE10" s="3">
         <v>0</v>
       </c>
+      <c r="BF10" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11">
+        <v>124</v>
+      </c>
+      <c r="C11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11">
         <v>0.38397624332593427</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>0.80570241691842903</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>0.72379283048739118</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>0.86155606407322649</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>0.72134565535895412</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>0.79223913850724093</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>0.93547208418591055</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>0.88197602315006185</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>0.93410683012259177</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>0.89504964340651649</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>0.92599826388888862</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>0.97153916211293256</v>
       </c>
-      <c r="O11">
-        <v>1</v>
-      </c>
       <c r="P11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -2678,7 +2745,7 @@
       <c r="X11">
         <v>0</v>
       </c>
-      <c r="Y11" s="3">
+      <c r="Y11">
         <v>0</v>
       </c>
       <c r="Z11" s="3">
@@ -2777,56 +2844,59 @@
       <c r="BE11" s="3">
         <v>0</v>
       </c>
+      <c r="BF11" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12">
+        <v>123</v>
+      </c>
+      <c r="C12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12">
         <v>0.36910994764397914</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>0.64090909090909109</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>0.21837893649974191</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>0.61751824817518275</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>0.21837893649974191</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>0.4976470588235295</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>0.53954081632653073</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>0.71452702702702697</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>0.64777947932618685</v>
       </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
       <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
         <v>0.94</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>0.58184319119669881</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>0.92763157894736858</v>
       </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
       <c r="Q12">
         <v>0</v>
       </c>
@@ -2851,7 +2921,7 @@
       <c r="X12">
         <v>0</v>
       </c>
-      <c r="Y12" s="3">
+      <c r="Y12">
         <v>0</v>
       </c>
       <c r="Z12" s="3">
@@ -2950,69 +3020,72 @@
       <c r="BE12" s="3">
         <v>0</v>
       </c>
+      <c r="BF12" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13">
-        <f>C12*C11</f>
+        <v>70</v>
+      </c>
+      <c r="C13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13">
+        <f>D12*D11</f>
         <v>0.14172945107056739</v>
       </c>
-      <c r="D13">
-        <f t="shared" ref="D13:O13" si="0">D12*D11</f>
+      <c r="E13">
+        <f>E12*E11</f>
         <v>0.51638200357044783</v>
       </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
+      <c r="F13">
+        <f t="shared" ref="E13:P13" si="0">F12*F11</f>
         <v>0.15806110856797445</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <f t="shared" si="0"/>
         <v>0.53202659139120434</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <f t="shared" si="0"/>
         <v>0.15752669706599776</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <f t="shared" si="0"/>
         <v>0.39425547716301523</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <f t="shared" si="0"/>
         <v>0.50472537195234723</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <f t="shared" si="0"/>
         <v>0.63019570573053396</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <f t="shared" si="0"/>
         <v>0.60509523605184734</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <f t="shared" si="0"/>
         <v>0.89504964340651649</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <f t="shared" si="0"/>
         <v>0.8704383680555553</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <f t="shared" si="0"/>
         <v>0.56528344645635553</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <f t="shared" si="0"/>
         <v>0.92763157894736858</v>
       </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
       <c r="Q13">
         <v>0</v>
       </c>
@@ -3037,7 +3110,7 @@
       <c r="X13">
         <v>0</v>
       </c>
-      <c r="Y13" s="3">
+      <c r="Y13">
         <v>0</v>
       </c>
       <c r="Z13" s="3">
@@ -3136,16 +3209,19 @@
       <c r="BE13" s="3">
         <v>0</v>
       </c>
+      <c r="BF13" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C14">
-        <v>1</v>
+      <c r="C14" t="s">
+        <v>89</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -3210,7 +3286,7 @@
       <c r="X14">
         <v>1</v>
       </c>
-      <c r="Y14" s="3">
+      <c r="Y14">
         <v>1</v>
       </c>
       <c r="Z14" s="3">
@@ -3244,7 +3320,7 @@
         <v>1</v>
       </c>
       <c r="AJ14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK14" s="3">
         <v>0</v>
@@ -3309,16 +3385,19 @@
       <c r="BE14" s="3">
         <v>0</v>
       </c>
+      <c r="BF14" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C15">
-        <v>1</v>
+      <c r="C15" t="s">
+        <v>89</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -3383,7 +3462,7 @@
       <c r="X15">
         <v>1</v>
       </c>
-      <c r="Y15" s="3">
+      <c r="Y15">
         <v>1</v>
       </c>
       <c r="Z15" s="3">
@@ -3417,7 +3496,7 @@
         <v>1</v>
       </c>
       <c r="AJ15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK15" s="3">
         <v>0</v>
@@ -3482,16 +3561,19 @@
       <c r="BE15" s="3">
         <v>0</v>
       </c>
+      <c r="BF15" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
+        <v>89</v>
+      </c>
+      <c r="C16" t="s">
+        <v>89</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -3556,7 +3638,7 @@
       <c r="X16">
         <v>1</v>
       </c>
-      <c r="Y16" s="3">
+      <c r="Y16">
         <v>1</v>
       </c>
       <c r="Z16" s="3">
@@ -3590,7 +3672,7 @@
         <v>1</v>
       </c>
       <c r="AJ16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK16" s="3">
         <v>0</v>
@@ -3655,16 +3737,19 @@
       <c r="BE16" s="3">
         <v>0</v>
       </c>
+      <c r="BF16" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
+        <v>126</v>
+      </c>
+      <c r="C17" t="s">
+        <v>131</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -3703,53 +3788,53 @@
         <v>0</v>
       </c>
       <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
         <v>0.64268377253814146</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>0.80868237347294936</v>
       </c>
-      <c r="R17">
+      <c r="S17">
         <v>0.74994942342706861</v>
       </c>
-      <c r="S17">
+      <c r="T17">
         <v>0.60561999673255995</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>0.79737577973757801</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <v>0.99383378016085788</v>
       </c>
-      <c r="V17">
-        <v>1</v>
-      </c>
       <c r="W17">
+        <v>1</v>
+      </c>
+      <c r="X17">
         <v>0.74919159256265155</v>
       </c>
-      <c r="X17">
+      <c r="Y17">
         <v>0.87656656419957435</v>
       </c>
-      <c r="Y17" s="3">
+      <c r="Z17" s="3">
         <v>0.27860696517412936</v>
       </c>
-      <c r="Z17" s="3">
-        <v>1</v>
-      </c>
       <c r="AA17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB17" s="3">
         <v>0.37583892617449666</v>
       </c>
-      <c r="AB17" s="3">
+      <c r="AC17" s="3">
         <v>0.40143369175627241</v>
       </c>
-      <c r="AC17" s="3">
+      <c r="AD17" s="3">
         <v>0.33234421364985162</v>
       </c>
-      <c r="AD17" s="3">
+      <c r="AE17" s="3">
         <v>0.56565656565656564</v>
       </c>
-      <c r="AE17" s="3">
-        <v>0</v>
-      </c>
       <c r="AF17" s="3">
         <v>0</v>
       </c>
@@ -3828,16 +3913,19 @@
       <c r="BE17" s="3">
         <v>0</v>
       </c>
+      <c r="BF17" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
+        <v>125</v>
+      </c>
+      <c r="C18" t="s">
+        <v>132</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -3876,53 +3964,53 @@
         <v>0</v>
       </c>
       <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
         <v>0.36322092656791682</v>
       </c>
-      <c r="Q18">
+      <c r="R18">
         <v>0.60546361964801676</v>
       </c>
-      <c r="R18">
+      <c r="S18">
         <v>0.4568880079286422</v>
       </c>
-      <c r="S18">
+      <c r="T18">
         <v>0.19287088946531672</v>
       </c>
-      <c r="T18">
+      <c r="U18">
         <v>0.59391909301726364</v>
       </c>
-      <c r="U18">
-        <v>1</v>
-      </c>
       <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="W18">
         <v>0.98884598884598884</v>
       </c>
-      <c r="W18">
+      <c r="X18">
         <v>0.53604651162790695</v>
       </c>
-      <c r="X18">
+      <c r="Y18">
         <v>0.86491557223264537</v>
       </c>
-      <c r="Y18" s="3">
+      <c r="Z18" s="3">
         <v>0.54216867469879515</v>
       </c>
-      <c r="Z18" s="3">
-        <v>1</v>
-      </c>
       <c r="AA18" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB18" s="3">
         <v>0.29315960912052119</v>
       </c>
-      <c r="AB18" s="3">
+      <c r="AC18" s="3">
         <v>0.30716723549488056</v>
       </c>
-      <c r="AC18" s="3">
+      <c r="AD18" s="3">
         <v>0.43902439024390244</v>
       </c>
-      <c r="AD18" s="3">
+      <c r="AE18" s="3">
         <v>0.36144578313253012</v>
       </c>
-      <c r="AE18" s="3">
-        <v>0</v>
-      </c>
       <c r="AF18" s="3">
         <v>0</v>
       </c>
@@ -4001,16 +4089,19 @@
       <c r="BE18" s="3">
         <v>0</v>
       </c>
+      <c r="BF18" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
+        <v>70</v>
+      </c>
+      <c r="C19" t="s">
+        <v>133</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -4049,53 +4140,53 @@
         <v>0</v>
       </c>
       <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
         <v>0.46468986111111099</v>
       </c>
-      <c r="Q19">
+      <c r="R19">
         <v>0.51031225694444438</v>
       </c>
-      <c r="R19">
+      <c r="S19">
         <v>0.52973999999999988</v>
       </c>
-      <c r="S19">
+      <c r="T19">
         <v>0.45403111111111122</v>
       </c>
-      <c r="T19">
+      <c r="U19">
         <v>0.52557581249999985</v>
-      </c>
-      <c r="U19">
-        <v>0.54629152777777779</v>
       </c>
       <c r="V19">
         <v>0.54629152777777779</v>
       </c>
       <c r="W19">
+        <v>0.54629152777777779</v>
+      </c>
+      <c r="X19">
         <v>0.36465800000000009</v>
       </c>
-      <c r="X19">
+      <c r="Y19">
         <v>0.54168452777777776</v>
       </c>
-      <c r="Y19" s="3">
+      <c r="Z19" s="3">
         <v>0.471655328798186</v>
       </c>
-      <c r="Z19" s="3">
-        <v>1</v>
-      </c>
       <c r="AA19" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB19" s="3">
         <v>0.53911564625850339</v>
       </c>
-      <c r="AB19" s="3">
+      <c r="AC19" s="3">
         <v>0.58106575963718821</v>
       </c>
-      <c r="AC19" s="3">
+      <c r="AD19" s="3">
         <v>0.55328798185941042</v>
       </c>
-      <c r="AD19" s="3">
+      <c r="AE19" s="3">
         <v>0.83730158730158721</v>
       </c>
-      <c r="AE19" s="3">
-        <v>0</v>
-      </c>
       <c r="AF19" s="3">
         <v>0</v>
       </c>
@@ -4174,16 +4265,19 @@
       <c r="BE19" s="3">
         <v>0</v>
       </c>
+      <c r="BF19" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C20">
-        <v>0</v>
+      <c r="C20" t="s">
+        <v>89</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -4248,8 +4342,8 @@
       <c r="X20">
         <v>0</v>
       </c>
-      <c r="Y20" s="3">
-        <v>1</v>
+      <c r="Y20">
+        <v>0</v>
       </c>
       <c r="Z20" s="3">
         <v>1</v>
@@ -4267,7 +4361,7 @@
         <v>1</v>
       </c>
       <c r="AE20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF20" s="3">
         <v>0</v>
@@ -4347,16 +4441,19 @@
       <c r="BE20" s="3">
         <v>0</v>
       </c>
+      <c r="BF20" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C21">
-        <v>0</v>
+      <c r="C21" t="s">
+        <v>134</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -4421,7 +4518,7 @@
       <c r="X21">
         <v>0</v>
       </c>
-      <c r="Y21" s="3">
+      <c r="Y21">
         <v>0</v>
       </c>
       <c r="Z21" s="3">
@@ -4440,23 +4537,23 @@
         <v>0</v>
       </c>
       <c r="AE21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="3">
         <v>0.97563025210084031</v>
       </c>
-      <c r="AF21" s="3">
-        <v>1</v>
-      </c>
       <c r="AG21" s="3">
+        <v>1</v>
+      </c>
+      <c r="AH21" s="3">
         <v>0.83697478991596641</v>
       </c>
-      <c r="AH21" s="3">
+      <c r="AI21" s="3">
         <v>0.754621848739496</v>
       </c>
-      <c r="AI21" s="3">
+      <c r="AJ21" s="3">
         <v>0.62016806722689077</v>
       </c>
-      <c r="AJ21" s="3">
-        <v>0</v>
-      </c>
       <c r="AK21" s="3">
         <v>0</v>
       </c>
@@ -4520,16 +4617,19 @@
       <c r="BE21" s="3">
         <v>0</v>
       </c>
+      <c r="BF21" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
+        <v>71</v>
+      </c>
+      <c r="C22" t="s">
+        <v>89</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -4594,7 +4694,7 @@
       <c r="X22">
         <v>0</v>
       </c>
-      <c r="Y22" s="3">
+      <c r="Y22">
         <v>0</v>
       </c>
       <c r="Z22" s="3">
@@ -4628,29 +4728,29 @@
         <v>0</v>
       </c>
       <c r="AJ22" s="3">
-        <v>1</v>
-      </c>
-      <c r="AK22">
+        <v>0</v>
+      </c>
+      <c r="AK22" s="3">
+        <v>1</v>
+      </c>
+      <c r="AL22">
         <v>0.77439797211660322</v>
       </c>
-      <c r="AL22">
+      <c r="AM22">
         <v>0.56147021546261078</v>
       </c>
-      <c r="AM22">
+      <c r="AN22">
         <v>0.83269961977186313</v>
       </c>
-      <c r="AN22">
+      <c r="AO22">
         <v>0.71482889733840294</v>
       </c>
-      <c r="AO22">
+      <c r="AP22">
         <v>0.94169835234474009</v>
       </c>
-      <c r="AP22">
+      <c r="AQ22">
         <v>0.64892268694550059</v>
       </c>
-      <c r="AQ22" s="3">
-        <v>0</v>
-      </c>
       <c r="AR22" s="3">
         <v>0</v>
       </c>
@@ -4693,16 +4793,19 @@
       <c r="BE22" s="3">
         <v>0</v>
       </c>
+      <c r="BF22" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
+        <v>72</v>
+      </c>
+      <c r="C23" t="s">
+        <v>120</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -4767,7 +4870,7 @@
       <c r="X23">
         <v>0</v>
       </c>
-      <c r="Y23" s="3">
+      <c r="Y23">
         <v>0</v>
       </c>
       <c r="Z23" s="3">
@@ -4821,30 +4924,30 @@
       <c r="AP23" s="3">
         <v>0</v>
       </c>
-      <c r="AQ23">
+      <c r="AQ23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AR23">
         <v>0.78797083839611193</v>
       </c>
-      <c r="AR23">
+      <c r="AS23">
         <v>0.81206966383151069</v>
       </c>
-      <c r="AS23">
+      <c r="AT23">
         <v>0.92831105710814099</v>
       </c>
-      <c r="AT23" s="3">
-        <v>1</v>
-      </c>
-      <c r="AU23">
+      <c r="AU23" s="3">
+        <v>1</v>
+      </c>
+      <c r="AV23">
         <v>0.98541919805589306</v>
       </c>
-      <c r="AV23">
+      <c r="AW23">
         <v>0.87140542729850157</v>
       </c>
-      <c r="AW23">
+      <c r="AX23">
         <v>0.89712434183880108</v>
       </c>
-      <c r="AX23" s="3">
-        <v>0</v>
-      </c>
       <c r="AY23" s="3">
         <v>0</v>
       </c>
@@ -4866,16 +4969,19 @@
       <c r="BE23" s="3">
         <v>0</v>
       </c>
+      <c r="BF23" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="C24" t="s">
+        <v>89</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -4940,7 +5046,7 @@
       <c r="X24">
         <v>0</v>
       </c>
-      <c r="Y24" s="3">
+      <c r="Y24">
         <v>0</v>
       </c>
       <c r="Z24" s="3">
@@ -5016,39 +5122,42 @@
         <v>0</v>
       </c>
       <c r="AX24" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY24" s="3">
+        <v>1</v>
+      </c>
+      <c r="AZ24" s="3">
         <v>0.8</v>
       </c>
-      <c r="AZ24" s="3">
+      <c r="BA24" s="3">
         <v>0.6</v>
       </c>
-      <c r="BA24" s="3">
+      <c r="BB24" s="3">
         <v>0.4</v>
       </c>
-      <c r="BB24" s="3">
+      <c r="BC24" s="3">
         <v>0.2</v>
       </c>
-      <c r="BC24" s="3">
-        <v>0</v>
-      </c>
       <c r="BD24" s="3">
         <v>0</v>
       </c>
       <c r="BE24" s="3">
         <v>0</v>
       </c>
+      <c r="BF24" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
+        <v>74</v>
+      </c>
+      <c r="C25" t="s">
+        <v>89</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -5113,7 +5222,7 @@
       <c r="X25">
         <v>0</v>
       </c>
-      <c r="Y25" s="3">
+      <c r="Y25">
         <v>0</v>
       </c>
       <c r="Z25" s="3">
@@ -5204,79 +5313,82 @@
         <v>0</v>
       </c>
       <c r="BC25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD25" s="3">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="BE25" s="3">
-        <v>0.2</v>
+        <v>0.7</v>
+      </c>
+      <c r="BF25" s="3">
+        <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26">
         <v>0.90489913544668577</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>0.46176470588235291</v>
       </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
       <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
         <v>0.48307692307692307</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>0.94864048338368567</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>2.3903775883069429E-2</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>6.7924201782469497E-3</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>0.60617760617760619</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>0.35885714285714282</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <v>0.18416422287390027</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <v>0.7302325581395348</v>
       </c>
-      <c r="N26">
+      <c r="O26">
         <v>0.59133709981167604</v>
       </c>
-      <c r="O26">
+      <c r="P26">
         <v>2.7689594356261022E-2</v>
       </c>
-      <c r="P26">
+      <c r="Q26">
         <v>0.9</v>
       </c>
-      <c r="Q26">
+      <c r="R26">
         <v>0.2</v>
       </c>
-      <c r="R26">
-        <v>1</v>
-      </c>
       <c r="S26">
+        <v>1</v>
+      </c>
+      <c r="T26">
         <v>0.4</v>
       </c>
-      <c r="T26">
+      <c r="U26">
         <v>0.3</v>
       </c>
-      <c r="U26">
-        <v>1</v>
-      </c>
       <c r="V26">
         <v>1</v>
       </c>
@@ -5284,86 +5396,86 @@
         <v>1</v>
       </c>
       <c r="X26">
+        <v>1</v>
+      </c>
+      <c r="Y26">
         <v>0.6</v>
       </c>
-      <c r="Y26" s="3">
+      <c r="Z26" s="3">
         <v>0.93243243243243235</v>
       </c>
-      <c r="Z26" s="3">
+      <c r="AA26" s="3">
         <v>0.34673366834170855</v>
       </c>
-      <c r="AA26" s="3">
+      <c r="AB26" s="3">
         <v>0.9078947368421052</v>
       </c>
-      <c r="AB26" s="3">
+      <c r="AC26" s="3">
         <v>0.50364963503649629</v>
       </c>
-      <c r="AC26" s="3">
+      <c r="AD26" s="3">
         <v>0.45695364238410596</v>
       </c>
-      <c r="AD26" s="3">
-        <v>1</v>
-      </c>
       <c r="AE26" s="3">
+        <v>1</v>
+      </c>
+      <c r="AF26" s="3">
         <v>0.68594306049822074</v>
       </c>
-      <c r="AF26" s="3">
+      <c r="AG26" s="3">
         <v>0.22456310679611652</v>
       </c>
-      <c r="AG26" s="3">
-        <v>1</v>
-      </c>
       <c r="AH26" s="3">
+        <v>1</v>
+      </c>
+      <c r="AI26" s="3">
         <v>0.41765980498374872</v>
       </c>
-      <c r="AI26" s="3">
+      <c r="AJ26" s="3">
         <v>0.42354880058597327</v>
       </c>
-      <c r="AJ26" s="3">
+      <c r="AK26" s="3">
         <v>0.05</v>
       </c>
-      <c r="AK26">
+      <c r="AL26">
         <v>0.6428571428571429</v>
       </c>
-      <c r="AL26">
+      <c r="AM26">
         <v>0.68</v>
       </c>
-      <c r="AM26">
+      <c r="AN26">
         <v>0.44285714285714284</v>
       </c>
-      <c r="AN26">
-        <v>1</v>
-      </c>
       <c r="AO26">
+        <v>1</v>
+      </c>
+      <c r="AP26">
         <v>0.21428571428571427</v>
       </c>
-      <c r="AP26">
+      <c r="AQ26">
         <v>0.41285714285714281</v>
       </c>
-      <c r="AQ26">
+      <c r="AR26">
         <v>0.88189541701567542</v>
       </c>
-      <c r="AR26">
+      <c r="AS26">
         <v>0.98397863818424569</v>
       </c>
-      <c r="AS26">
+      <c r="AT26">
         <v>0.32770120053357049</v>
       </c>
-      <c r="AT26" s="3">
-        <v>1</v>
-      </c>
-      <c r="AU26">
+      <c r="AU26" s="3">
+        <v>1</v>
+      </c>
+      <c r="AV26">
         <v>5.0125824661633678E-2</v>
       </c>
-      <c r="AV26">
+      <c r="AW26">
         <v>0.63644214162348878</v>
       </c>
-      <c r="AW26">
+      <c r="AX26">
         <v>0.17353425947727807</v>
       </c>
-      <c r="AX26" s="3">
-        <v>1</v>
-      </c>
       <c r="AY26" s="3">
         <v>1</v>
       </c>
@@ -5385,89 +5497,91 @@
       <c r="BE26" s="3">
         <v>1</v>
       </c>
+      <c r="BF26" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="27" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27">
-        <f>C26*C13</f>
+        <v>76</v>
+      </c>
+      <c r="C27" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27">
+        <f>D26*D13</f>
         <v>0.1282508577410898</v>
       </c>
-      <c r="D27">
-        <f t="shared" ref="D27:O27" si="1">D26*D13</f>
+      <c r="E27">
+        <f t="shared" ref="E27:P27" si="1">E26*E13</f>
         <v>0.23844698400164796</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <f t="shared" si="1"/>
         <v>0.15806110856797445</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <f t="shared" si="1"/>
         <v>0.25700976876436638</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <f t="shared" si="1"/>
         <v>0.14943620205052352</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <f t="shared" si="1"/>
         <v>9.4241945667773129E-3</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <f t="shared" si="1"/>
         <v>3.4283068009223205E-3</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <f t="shared" si="1"/>
         <v>0.3820105243231422</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <f t="shared" si="1"/>
         <v>0.21714274756603433</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <f t="shared" si="1"/>
         <v>0.16483612201152267</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <f t="shared" si="1"/>
         <v>0.63562243620801007</v>
       </c>
-      <c r="N27">
+      <c r="O27">
         <f t="shared" si="1"/>
         <v>0.33427307379905014</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <f t="shared" si="1"/>
         <v>2.5685742133110558E-2</v>
       </c>
-      <c r="P27">
-        <f t="shared" ref="P27:AC27" si="2">P26*P28</f>
-        <v>0.41822087500000005</v>
-      </c>
       <c r="Q27">
+        <f t="shared" ref="Q27:AD27" si="2">Q26*Q28</f>
+        <v>0.41822087499999988</v>
+      </c>
+      <c r="R27">
         <f t="shared" si="2"/>
         <v>0.10206245138888888</v>
       </c>
-      <c r="R27">
+      <c r="S27">
         <f t="shared" si="2"/>
         <v>0.52973999999999988</v>
       </c>
-      <c r="S27">
+      <c r="T27">
         <f t="shared" si="2"/>
         <v>0.18161244444444449</v>
       </c>
-      <c r="T27">
+      <c r="U27">
         <f t="shared" si="2"/>
         <v>0.15767274374999996</v>
-      </c>
-      <c r="U27">
-        <f t="shared" si="2"/>
-        <v>0.54629152777777779</v>
       </c>
       <c r="V27">
         <f t="shared" si="2"/>
@@ -5475,115 +5589,116 @@
       </c>
       <c r="W27">
         <f t="shared" si="2"/>
-        <v>0.36465800000000009</v>
+        <v>0.54629152777777779</v>
       </c>
       <c r="X27">
         <f t="shared" si="2"/>
-        <v>0.32501071666666664</v>
+        <v>0.36465800000000009</v>
       </c>
       <c r="Y27">
         <f t="shared" si="2"/>
-        <v>0.43978672550101122</v>
+        <v>0.32501071666666664</v>
       </c>
       <c r="Z27">
         <f t="shared" si="2"/>
-        <v>0.34673366834170855</v>
+        <v>0.43978672550101122</v>
       </c>
       <c r="AA27">
         <f t="shared" si="2"/>
-        <v>0.48946025778732544</v>
+        <v>0.34673366834170855</v>
       </c>
       <c r="AB27">
         <f t="shared" si="2"/>
-        <v>0.29265355777347429</v>
+        <v>0.48946025778732544</v>
       </c>
       <c r="AC27">
         <f t="shared" si="2"/>
+        <v>0.29265355777347429</v>
+      </c>
+      <c r="AD27">
+        <f t="shared" si="2"/>
         <v>0.25282695859800874</v>
       </c>
-      <c r="AD27">
-        <f t="shared" ref="AD27:AI27" si="3">AD26*AD28</f>
+      <c r="AE27">
+        <f t="shared" ref="AE27:AJ27" si="3">AE26*AE28</f>
         <v>0.83730158730158721</v>
       </c>
-      <c r="AE27">
+      <c r="AF27">
         <f t="shared" si="3"/>
         <v>0.66922680104070109</v>
       </c>
-      <c r="AF27">
+      <c r="AG27">
         <f t="shared" si="3"/>
         <v>0.22456310679611652</v>
       </c>
-      <c r="AG27">
+      <c r="AH27">
         <f t="shared" si="3"/>
         <v>0.83697478991596641</v>
       </c>
-      <c r="AH27">
+      <c r="AI27">
         <f t="shared" si="3"/>
         <v>0.3151752141810138</v>
       </c>
-      <c r="AI27">
+      <c r="AJ27">
         <f t="shared" si="3"/>
         <v>0.26267144103567081</v>
       </c>
-      <c r="AJ27">
-        <f t="shared" ref="AJ27:AP27" si="4">AJ26*AJ28</f>
+      <c r="AK27">
+        <f t="shared" ref="AK27:AQ27" si="4">AK26*AK28</f>
         <v>0.05</v>
       </c>
-      <c r="AK27">
+      <c r="AL27">
         <f t="shared" si="4"/>
         <v>0.49782726778924496</v>
       </c>
-      <c r="AL27">
+      <c r="AM27">
         <f t="shared" si="4"/>
         <v>0.38179974651457538</v>
       </c>
-      <c r="AM27">
+      <c r="AN27">
         <f t="shared" si="4"/>
         <v>0.36876697447039652</v>
       </c>
-      <c r="AN27">
+      <c r="AO27">
         <f t="shared" si="4"/>
         <v>0.71482889733840294</v>
       </c>
-      <c r="AO27">
+      <c r="AP27">
         <f t="shared" si="4"/>
         <v>0.20179250407387286</v>
       </c>
-      <c r="AP27">
+      <c r="AQ27">
         <f t="shared" si="4"/>
         <v>0.2679123664674995</v>
       </c>
-      <c r="AQ27">
-        <f t="shared" ref="AQ27" si="5">AQ26*AQ28</f>
+      <c r="AR27">
+        <f t="shared" ref="AR27" si="5">AR26*AR28</f>
         <v>0.69490787112353047</v>
       </c>
-      <c r="AR27">
-        <f t="shared" ref="AR27" si="6">AR26*AR28</f>
+      <c r="AS27">
+        <f t="shared" ref="AS27" si="6">AS26*AS28</f>
         <v>0.79905920192766811</v>
       </c>
-      <c r="AS27">
-        <f t="shared" ref="AS27" si="7">AS26*AS28</f>
+      <c r="AT27">
+        <f t="shared" ref="AT27" si="7">AT26*AT28</f>
         <v>0.30420864788292573</v>
       </c>
-      <c r="AT27">
-        <f t="shared" ref="AT27" si="8">AT26*AT28</f>
-        <v>1</v>
-      </c>
       <c r="AU27">
-        <f t="shared" ref="AU27" si="9">AU26*AU28</f>
+        <f t="shared" ref="AU27" si="8">AU26*AU28</f>
+        <v>1</v>
+      </c>
+      <c r="AV27">
+        <f t="shared" ref="AV27" si="9">AV26*AV28</f>
         <v>4.9394949939957369E-2</v>
       </c>
-      <c r="AV27">
-        <f t="shared" ref="AV27" si="10">AV26*AV28</f>
+      <c r="AW27">
+        <f t="shared" ref="AW27" si="10">AW26*AW28</f>
         <v>0.55459913637218972</v>
       </c>
-      <c r="AW27">
-        <f t="shared" ref="AW27" si="11">AW26*AW28</f>
+      <c r="AX27">
+        <f t="shared" ref="AX27" si="11">AX26*AX28</f>
         <v>0.15568180832003681</v>
       </c>
-      <c r="AX27" s="3">
-        <v>1</v>
-      </c>
       <c r="AY27" s="3">
         <v>1</v>
       </c>
@@ -5605,190 +5720,193 @@
       <c r="BE27" s="3">
         <v>1</v>
       </c>
+      <c r="BF27" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="28" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C28">
-        <f>C13</f>
+        <v>77</v>
+      </c>
+      <c r="C28" t="s">
+        <v>129</v>
+      </c>
+      <c r="D28">
+        <f>D13</f>
         <v>0.14172945107056739</v>
       </c>
-      <c r="D28">
-        <f t="shared" ref="D28:O28" si="12">D13</f>
+      <c r="E28">
+        <f t="shared" ref="E28:P28" si="12">E13</f>
         <v>0.51638200357044783</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <f t="shared" si="12"/>
         <v>0.15806110856797445</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <f t="shared" si="12"/>
         <v>0.53202659139120434</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <f t="shared" si="12"/>
         <v>0.15752669706599776</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <f t="shared" si="12"/>
         <v>0.39425547716301523</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <f t="shared" si="12"/>
         <v>0.50472537195234723</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <f t="shared" si="12"/>
         <v>0.63019570573053396</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <f t="shared" si="12"/>
         <v>0.60509523605184734</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <f t="shared" si="12"/>
         <v>0.89504964340651649</v>
       </c>
-      <c r="M28">
+      <c r="N28">
         <f t="shared" si="12"/>
         <v>0.8704383680555553</v>
       </c>
-      <c r="N28">
+      <c r="O28">
         <f t="shared" si="12"/>
         <v>0.56528344645635553</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <f t="shared" si="12"/>
         <v>0.92763157894736858</v>
       </c>
-      <c r="P28">
-        <v>0.46468986111111116</v>
-      </c>
       <c r="Q28">
+        <v>0.46468986111111099</v>
+      </c>
+      <c r="R28">
         <v>0.51031225694444438</v>
       </c>
-      <c r="R28">
+      <c r="S28">
         <v>0.52973999999999988</v>
       </c>
-      <c r="S28">
+      <c r="T28">
         <v>0.45403111111111122</v>
       </c>
-      <c r="T28">
+      <c r="U28">
         <v>0.52557581249999985</v>
-      </c>
-      <c r="U28">
-        <v>0.54629152777777779</v>
       </c>
       <c r="V28">
         <v>0.54629152777777779</v>
       </c>
       <c r="W28">
+        <v>0.54629152777777779</v>
+      </c>
+      <c r="X28">
         <v>0.36465800000000009</v>
       </c>
-      <c r="X28">
+      <c r="Y28">
         <v>0.54168452777777776</v>
       </c>
-      <c r="Y28" s="3">
+      <c r="Z28" s="3">
         <v>0.471655328798186</v>
       </c>
-      <c r="Z28" s="3">
-        <v>1</v>
-      </c>
       <c r="AA28" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB28" s="3">
         <v>0.53911564625850339</v>
       </c>
-      <c r="AB28" s="3">
+      <c r="AC28" s="3">
         <v>0.58106575963718821</v>
       </c>
-      <c r="AC28" s="3">
+      <c r="AD28" s="3">
         <v>0.55328798185941042</v>
       </c>
-      <c r="AD28" s="3">
+      <c r="AE28" s="3">
         <v>0.83730158730158721</v>
       </c>
-      <c r="AE28" s="3">
-        <f>AE21</f>
+      <c r="AF28" s="3">
+        <f>AF21</f>
         <v>0.97563025210084031</v>
       </c>
-      <c r="AF28" s="3">
-        <f t="shared" ref="AF28:AI28" si="13">AF21</f>
-        <v>1</v>
-      </c>
       <c r="AG28" s="3">
+        <f t="shared" ref="AG28:AJ28" si="13">AG21</f>
+        <v>1</v>
+      </c>
+      <c r="AH28" s="3">
         <f t="shared" si="13"/>
         <v>0.83697478991596641</v>
       </c>
-      <c r="AH28" s="3">
+      <c r="AI28" s="3">
         <f t="shared" si="13"/>
         <v>0.754621848739496</v>
       </c>
-      <c r="AI28" s="3">
+      <c r="AJ28" s="3">
         <f t="shared" si="13"/>
         <v>0.62016806722689077</v>
       </c>
-      <c r="AJ28">
-        <f>AJ22</f>
-        <v>1</v>
-      </c>
       <c r="AK28">
-        <f t="shared" ref="AK28:AP28" si="14">AK22</f>
+        <f>AK22</f>
+        <v>1</v>
+      </c>
+      <c r="AL28">
+        <f t="shared" ref="AL28:AQ28" si="14">AL22</f>
         <v>0.77439797211660322</v>
       </c>
-      <c r="AL28">
+      <c r="AM28">
         <f t="shared" si="14"/>
         <v>0.56147021546261078</v>
       </c>
-      <c r="AM28">
+      <c r="AN28">
         <f t="shared" si="14"/>
         <v>0.83269961977186313</v>
       </c>
-      <c r="AN28">
+      <c r="AO28">
         <f t="shared" si="14"/>
         <v>0.71482889733840294</v>
       </c>
-      <c r="AO28">
+      <c r="AP28">
         <f t="shared" si="14"/>
         <v>0.94169835234474009</v>
       </c>
-      <c r="AP28">
+      <c r="AQ28">
         <f t="shared" si="14"/>
         <v>0.64892268694550059</v>
       </c>
-      <c r="AQ28">
-        <f>AQ23</f>
+      <c r="AR28">
+        <f>AR23</f>
         <v>0.78797083839611193</v>
       </c>
-      <c r="AR28">
-        <f t="shared" ref="AR28:AW28" si="15">AR23</f>
+      <c r="AS28">
+        <f t="shared" ref="AS28:AX28" si="15">AS23</f>
         <v>0.81206966383151069</v>
       </c>
-      <c r="AS28">
+      <c r="AT28">
         <f t="shared" si="15"/>
         <v>0.92831105710814099</v>
       </c>
-      <c r="AT28">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
       <c r="AU28">
         <f t="shared" si="15"/>
-        <v>0.98541919805589306</v>
+        <v>1</v>
       </c>
       <c r="AV28">
         <f t="shared" si="15"/>
-        <v>0.87140542729850157</v>
+        <v>0.98541919805589306</v>
       </c>
       <c r="AW28">
         <f t="shared" si="15"/>
+        <v>0.87140542729850157</v>
+      </c>
+      <c r="AX28">
+        <f t="shared" si="15"/>
         <v>0.89712434183880108</v>
       </c>
-      <c r="AX28" s="3">
-        <v>1</v>
-      </c>
       <c r="AY28" s="3">
         <v>1</v>
       </c>
@@ -5810,16 +5928,19 @@
       <c r="BE28" s="3">
         <v>1</v>
       </c>
+      <c r="BF28" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="29" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C29">
-        <v>1</v>
+      <c r="C29" t="s">
+        <v>89</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -5884,7 +6005,7 @@
       <c r="X29">
         <v>1</v>
       </c>
-      <c r="Y29" s="3">
+      <c r="Y29">
         <v>1</v>
       </c>
       <c r="Z29" s="3">
@@ -5983,16 +6104,19 @@
       <c r="BE29" s="3">
         <v>1</v>
       </c>
+      <c r="BF29" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="30" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C30">
-        <v>1</v>
+      <c r="C30" t="s">
+        <v>89</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -6057,7 +6181,7 @@
       <c r="X30">
         <v>1</v>
       </c>
-      <c r="Y30" s="3">
+      <c r="Y30">
         <v>1</v>
       </c>
       <c r="Z30" s="3">
@@ -6156,16 +6280,19 @@
       <c r="BE30" s="3">
         <v>1</v>
       </c>
+      <c r="BF30" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="31" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="C31" t="s">
+        <v>89</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -6230,7 +6357,7 @@
       <c r="X31">
         <v>1</v>
       </c>
-      <c r="Y31" s="3">
+      <c r="Y31">
         <v>1</v>
       </c>
       <c r="Z31" s="3">
@@ -6329,16 +6456,19 @@
       <c r="BE31" s="3">
         <v>1</v>
       </c>
+      <c r="BF31" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="32" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
+        <v>79</v>
+      </c>
+      <c r="C32" t="s">
+        <v>89</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -6403,7 +6533,7 @@
       <c r="X32">
         <v>1</v>
       </c>
-      <c r="Y32" s="3">
+      <c r="Y32">
         <v>1</v>
       </c>
       <c r="Z32" s="3">
@@ -6502,16 +6632,19 @@
       <c r="BE32" s="3">
         <v>1</v>
       </c>
+      <c r="BF32" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="33" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="C33" t="s">
+        <v>89</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -6576,7 +6709,7 @@
       <c r="X33">
         <v>1</v>
       </c>
-      <c r="Y33" s="3">
+      <c r="Y33">
         <v>1</v>
       </c>
       <c r="Z33" s="3">
@@ -6675,16 +6808,19 @@
       <c r="BE33" s="3">
         <v>1</v>
       </c>
+      <c r="BF33" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="34" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
+        <v>81</v>
+      </c>
+      <c r="C34" t="s">
+        <v>89</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -6749,7 +6885,7 @@
       <c r="X34">
         <v>1</v>
       </c>
-      <c r="Y34" s="3">
+      <c r="Y34">
         <v>1</v>
       </c>
       <c r="Z34" s="3">
@@ -6848,16 +6984,19 @@
       <c r="BE34" s="3">
         <v>1</v>
       </c>
+      <c r="BF34" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="35" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
+        <v>82</v>
+      </c>
+      <c r="C35" t="s">
+        <v>89</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -6922,7 +7061,7 @@
       <c r="X35">
         <v>1</v>
       </c>
-      <c r="Y35" s="3">
+      <c r="Y35">
         <v>1</v>
       </c>
       <c r="Z35" s="3">
@@ -7021,16 +7160,19 @@
       <c r="BE35" s="3">
         <v>1</v>
       </c>
+      <c r="BF35" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="36" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
+        <v>83</v>
+      </c>
+      <c r="C36" t="s">
+        <v>89</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -7095,7 +7237,7 @@
       <c r="X36">
         <v>1</v>
       </c>
-      <c r="Y36" s="3">
+      <c r="Y36">
         <v>1</v>
       </c>
       <c r="Z36" s="3">
@@ -7194,16 +7336,19 @@
       <c r="BE36" s="3">
         <v>1</v>
       </c>
+      <c r="BF36" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37">
-        <v>1</v>
+        <v>84</v>
+      </c>
+      <c r="C37" t="s">
+        <v>89</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -7268,7 +7413,7 @@
       <c r="X37">
         <v>1</v>
       </c>
-      <c r="Y37" s="3">
+      <c r="Y37">
         <v>1</v>
       </c>
       <c r="Z37" s="3">
@@ -7367,17 +7512,20 @@
       <c r="BE37" s="3">
         <v>1</v>
       </c>
+      <c r="BF37" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="38" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" t="s">
         <v>89</v>
       </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
       <c r="D38">
         <v>1</v>
       </c>
@@ -7441,7 +7589,7 @@
       <c r="X38">
         <v>1</v>
       </c>
-      <c r="Y38" s="3">
+      <c r="Y38">
         <v>1</v>
       </c>
       <c r="Z38" s="3">
@@ -7540,16 +7688,19 @@
       <c r="BE38" s="3">
         <v>1</v>
       </c>
+      <c r="BF38" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="39" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
+        <v>86</v>
+      </c>
+      <c r="C39" t="s">
+        <v>89</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -7614,7 +7765,7 @@
       <c r="X39">
         <v>1</v>
       </c>
-      <c r="Y39" s="3">
+      <c r="Y39">
         <v>1</v>
       </c>
       <c r="Z39" s="3">
@@ -7713,16 +7864,19 @@
       <c r="BE39" s="3">
         <v>1</v>
       </c>
+      <c r="BF39" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="40" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
+        <v>87</v>
+      </c>
+      <c r="C40" t="s">
+        <v>89</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -7787,7 +7941,7 @@
       <c r="X40">
         <v>1</v>
       </c>
-      <c r="Y40" s="3">
+      <c r="Y40">
         <v>1</v>
       </c>
       <c r="Z40" s="3">
@@ -7886,16 +8040,19 @@
       <c r="BE40" s="3">
         <v>1</v>
       </c>
+      <c r="BF40" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="41" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="C41" t="s">
+        <v>89</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -7960,7 +8117,7 @@
       <c r="X41">
         <v>1</v>
       </c>
-      <c r="Y41" s="3">
+      <c r="Y41">
         <v>1</v>
       </c>
       <c r="Z41" s="3">
@@ -8057,6 +8214,9 @@
         <v>1</v>
       </c>
       <c r="BE41" s="3">
+        <v>1</v>
+      </c>
+      <c r="BF41" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>